<commit_message>
UPDATE assignment 5, data consolidated
</commit_message>
<xml_diff>
--- a/data/mediciones-hojas.xlsx
+++ b/data/mediciones-hojas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="false" showVerticalScroll="false" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="17">
   <si>
-    <t xml:space="preserve">individuo-grupo</t>
+    <t xml:space="preserve">grupo</t>
   </si>
   <si>
     <t xml:space="preserve">mediciones hechas por</t>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">id de hoja</t>
   </si>
   <si>
-    <t xml:space="preserve">estudiante</t>
+    <t xml:space="preserve">colectas hechas por</t>
   </si>
   <si>
-    <t xml:space="preserve">ancho</t>
+    <t xml:space="preserve">ancho (cm)</t>
   </si>
   <si>
-    <t xml:space="preserve">largo</t>
+    <t xml:space="preserve">largo (cm)</t>
   </si>
   <si>
     <t xml:space="preserve">Melany, María y Aironeli</t>
@@ -85,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -172,29 +173,29 @@
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="false" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E82" activeCellId="0" sqref="E82:F101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -202,19 +203,19 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>7.3</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>14</v>
       </c>
     </row>
@@ -225,16 +226,16 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>7.8</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>14.2</v>
       </c>
     </row>
@@ -245,16 +246,16 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>9.6</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>18.4</v>
       </c>
     </row>
@@ -265,16 +266,16 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>8.1</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>14.2</v>
       </c>
     </row>
@@ -285,16 +286,16 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>6.9</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>15.4</v>
       </c>
     </row>
@@ -305,16 +306,16 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>18.5</v>
       </c>
     </row>
@@ -325,16 +326,16 @@
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>7.6</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>17</v>
       </c>
     </row>
@@ -345,16 +346,16 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>6.6</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -365,16 +366,16 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>7.7</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>17.1</v>
       </c>
     </row>
@@ -385,16 +386,16 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>7.6</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>15.4</v>
       </c>
     </row>
@@ -405,16 +406,16 @@
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D12" s="0" t="s">
+      <c r="C12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>16.3</v>
       </c>
     </row>
@@ -425,16 +426,16 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="C13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>17.6</v>
       </c>
     </row>
@@ -445,16 +446,16 @@
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="C14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>15</v>
       </c>
     </row>
@@ -465,16 +466,16 @@
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="C15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>17</v>
       </c>
     </row>
@@ -485,16 +486,16 @@
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="C16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>6.3</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>14.8</v>
       </c>
     </row>
@@ -505,16 +506,16 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="C17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>5.5</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>11.9</v>
       </c>
     </row>
@@ -525,16 +526,16 @@
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>16.8</v>
       </c>
     </row>
@@ -545,16 +546,16 @@
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>15.9</v>
       </c>
     </row>
@@ -565,16 +566,16 @@
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>8.2</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>17.2</v>
       </c>
     </row>
@@ -585,16 +586,16 @@
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>6.3</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>13</v>
       </c>
     </row>
@@ -602,19 +603,19 @@
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="0" t="n">
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>7.5</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>14.3</v>
       </c>
     </row>
@@ -625,16 +626,16 @@
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>15.7</v>
       </c>
     </row>
@@ -645,16 +646,16 @@
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>9.4</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>18.5</v>
       </c>
     </row>
@@ -665,16 +666,16 @@
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>8.1</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>14.6</v>
       </c>
     </row>
@@ -685,16 +686,16 @@
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -705,16 +706,16 @@
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>18.4</v>
       </c>
     </row>
@@ -725,16 +726,16 @@
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>7.6</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <v>17.1</v>
       </c>
     </row>
@@ -745,16 +746,16 @@
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <v>12.1</v>
       </c>
     </row>
@@ -765,16 +766,16 @@
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>7.4</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <v>17.3</v>
       </c>
     </row>
@@ -785,16 +786,16 @@
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>7.6</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -805,16 +806,16 @@
       <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="C32" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>7.4</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <v>16.2</v>
       </c>
     </row>
@@ -825,16 +826,16 @@
       <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="C33" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>8.2</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <v>17.6</v>
       </c>
     </row>
@@ -845,16 +846,16 @@
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D34" s="0" t="s">
+      <c r="C34" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>15.2</v>
       </c>
     </row>
@@ -865,16 +866,16 @@
       <c r="B35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="C35" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>8.9</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="1" t="n">
         <v>17.1</v>
       </c>
     </row>
@@ -885,16 +886,16 @@
       <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D36" s="0" t="s">
+      <c r="C36" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>6.3</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>15</v>
       </c>
     </row>
@@ -905,16 +906,16 @@
       <c r="B37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D37" s="0" t="s">
+      <c r="C37" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>6.6</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -925,16 +926,16 @@
       <c r="B38" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38" s="1" t="n">
         <v>16.7</v>
       </c>
     </row>
@@ -945,16 +946,16 @@
       <c r="B39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>7.6</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39" s="1" t="n">
         <v>16</v>
       </c>
     </row>
@@ -965,16 +966,16 @@
       <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="1" t="n">
         <v>17.3</v>
       </c>
     </row>
@@ -985,16 +986,16 @@
       <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>6.2</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="1" t="n">
         <v>13.1</v>
       </c>
     </row>
@@ -1005,16 +1006,16 @@
       <c r="B42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="0" t="n">
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="1" t="n">
         <v>24.4</v>
       </c>
     </row>
@@ -1025,16 +1026,16 @@
       <c r="B43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="0" t="n">
+      <c r="D43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1" t="n">
         <v>9.5</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="1" t="n">
         <v>20.7</v>
       </c>
     </row>
@@ -1045,16 +1046,16 @@
       <c r="B44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="0" t="n">
+      <c r="D44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1" t="n">
         <v>9.2</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="1" t="n">
         <v>24.2</v>
       </c>
     </row>
@@ -1065,16 +1066,16 @@
       <c r="B45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="0" t="n">
+      <c r="D45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="1" t="n">
         <v>23.3</v>
       </c>
     </row>
@@ -1085,16 +1086,16 @@
       <c r="B46" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="0" t="n">
+      <c r="D46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1" t="n">
         <v>9.4</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="1" t="n">
         <v>25.7</v>
       </c>
     </row>
@@ -1105,16 +1106,16 @@
       <c r="B47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="0" t="n">
+      <c r="C47" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1" t="n">
         <v>8.1</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="1" t="n">
         <v>22.7</v>
       </c>
     </row>
@@ -1125,16 +1126,16 @@
       <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="0" t="n">
+      <c r="D48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="1" t="n">
         <v>10.8</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="1" t="n">
         <v>29.6</v>
       </c>
     </row>
@@ -1145,16 +1146,16 @@
       <c r="B49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="0" t="n">
+      <c r="C49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49" s="1" t="n">
         <v>28.6</v>
       </c>
     </row>
@@ -1165,16 +1166,16 @@
       <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="0" t="n">
+      <c r="D50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1" t="n">
         <v>10.8</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50" s="1" t="n">
         <v>29.7</v>
       </c>
     </row>
@@ -1185,16 +1186,16 @@
       <c r="B51" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="0" t="n">
+      <c r="D51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="1" t="n">
         <v>6.9</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="1" t="n">
         <v>19.6</v>
       </c>
     </row>
@@ -1205,16 +1206,16 @@
       <c r="B52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="0" t="n">
+      <c r="C52" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="1" t="n">
         <v>9.1</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="F52" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1225,16 +1226,16 @@
       <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="0" t="n">
+      <c r="C53" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1" t="n">
         <v>9.6</v>
       </c>
-      <c r="F53" s="0" t="n">
+      <c r="F53" s="1" t="n">
         <v>29.1</v>
       </c>
     </row>
@@ -1245,16 +1246,16 @@
       <c r="B54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" s="0" t="n">
+      <c r="C54" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1" t="n">
         <v>8.6</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F54" s="1" t="n">
         <v>22.1</v>
       </c>
     </row>
@@ -1265,16 +1266,16 @@
       <c r="B55" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F55" s="0" t="n">
+      <c r="C55" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F55" s="1" t="n">
         <v>25.9</v>
       </c>
     </row>
@@ -1285,16 +1286,16 @@
       <c r="B56" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="0" t="n">
+      <c r="C56" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="F56" s="0" t="n">
+      <c r="F56" s="1" t="n">
         <v>29.3</v>
       </c>
     </row>
@@ -1305,16 +1306,16 @@
       <c r="B57" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="0" t="n">
+      <c r="C57" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="1" t="n">
         <v>9.1</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="F57" s="1" t="n">
         <v>23.8</v>
       </c>
     </row>
@@ -1325,16 +1326,16 @@
       <c r="B58" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="0" t="n">
+      <c r="D58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58" s="1" t="n">
         <v>23.9</v>
       </c>
     </row>
@@ -1345,16 +1346,16 @@
       <c r="B59" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="0" t="n">
+      <c r="D59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1" t="n">
         <v>8.8</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="F59" s="1" t="n">
         <v>25.6</v>
       </c>
     </row>
@@ -1365,16 +1366,16 @@
       <c r="B60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="0" t="n">
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="1" t="n">
         <v>10.5</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="F60" s="1" t="n">
         <v>29.2</v>
       </c>
     </row>
@@ -1385,16 +1386,16 @@
       <c r="B61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="0" t="n">
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="1" t="n">
         <v>12.1</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F61" s="1" t="n">
         <v>30.1</v>
       </c>
     </row>
@@ -1405,16 +1406,16 @@
       <c r="B62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="0" t="n">
+      <c r="D62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="1" t="n">
         <v>9.7</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62" s="1" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1425,16 +1426,16 @@
       <c r="B63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="0" t="n">
+      <c r="D63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63" s="1" t="n">
         <v>27.3</v>
       </c>
     </row>
@@ -1445,16 +1446,16 @@
       <c r="B64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="0" t="n">
+      <c r="D64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="1" t="n">
         <v>9.5</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64" s="1" t="n">
         <v>24.8</v>
       </c>
     </row>
@@ -1465,16 +1466,16 @@
       <c r="B65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="0" t="n">
+      <c r="D65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="1" t="n">
         <v>9.3</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65" s="1" t="n">
         <v>23.5</v>
       </c>
     </row>
@@ -1485,16 +1486,16 @@
       <c r="B66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="0" t="n">
+      <c r="D66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="1" t="n">
         <v>9.9</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="1" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1505,16 +1506,16 @@
       <c r="B67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="0" t="n">
+      <c r="C67" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="1" t="n">
         <v>8.3</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="F67" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1525,16 +1526,16 @@
       <c r="B68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="0" t="n">
+      <c r="D68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="1" t="n">
         <v>10.9</v>
       </c>
-      <c r="F68" s="0" t="n">
+      <c r="F68" s="1" t="n">
         <v>30</v>
       </c>
     </row>
@@ -1545,16 +1546,16 @@
       <c r="B69" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="0" t="n">
+      <c r="C69" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="1" t="n">
         <v>10.3</v>
       </c>
-      <c r="F69" s="0" t="n">
+      <c r="F69" s="1" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1565,16 +1566,16 @@
       <c r="B70" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D70" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F70" s="0" t="n">
+      <c r="D70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="F70" s="1" t="n">
         <v>30.5</v>
       </c>
     </row>
@@ -1585,16 +1586,16 @@
       <c r="B71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D71" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="0" t="n">
+      <c r="D71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="1" t="n">
         <v>6.8</v>
       </c>
-      <c r="F71" s="0" t="n">
+      <c r="F71" s="1" t="n">
         <v>20.2</v>
       </c>
     </row>
@@ -1605,16 +1606,16 @@
       <c r="B72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" s="0" t="n">
+      <c r="C72" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="1" t="n">
         <v>9.3</v>
       </c>
-      <c r="F72" s="0" t="n">
+      <c r="F72" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1625,16 +1626,16 @@
       <c r="B73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="0" t="n">
+      <c r="C73" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="1" t="n">
         <v>10.1</v>
       </c>
-      <c r="F73" s="0" t="n">
+      <c r="F73" s="1" t="n">
         <v>26.5</v>
       </c>
     </row>
@@ -1645,16 +1646,16 @@
       <c r="B74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E74" s="0" t="n">
+      <c r="C74" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="1" t="n">
         <v>8.7</v>
       </c>
-      <c r="F74" s="0" t="n">
+      <c r="F74" s="1" t="n">
         <v>22.2</v>
       </c>
     </row>
@@ -1665,16 +1666,16 @@
       <c r="B75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C75" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" s="0" t="n">
+      <c r="C75" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="1" t="n">
         <v>9.2</v>
       </c>
-      <c r="F75" s="0" t="n">
+      <c r="F75" s="1" t="n">
         <v>26.2</v>
       </c>
     </row>
@@ -1685,16 +1686,16 @@
       <c r="B76" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E76" s="0" t="n">
+      <c r="C76" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="1" t="n">
         <v>11.7</v>
       </c>
-      <c r="F76" s="0" t="n">
+      <c r="F76" s="1" t="n">
         <v>29.3</v>
       </c>
     </row>
@@ -1705,16 +1706,16 @@
       <c r="B77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E77" s="0" t="n">
+      <c r="C77" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="1" t="n">
         <v>9.3</v>
       </c>
-      <c r="F77" s="0" t="n">
+      <c r="F77" s="1" t="n">
         <v>24.2</v>
       </c>
     </row>
@@ -1725,16 +1726,16 @@
       <c r="B78" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="C78" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D78" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E78" s="0" t="n">
+      <c r="D78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="1" t="n">
         <v>9.1</v>
       </c>
-      <c r="F78" s="0" t="n">
+      <c r="F78" s="1" t="n">
         <v>24.3</v>
       </c>
     </row>
@@ -1745,16 +1746,16 @@
       <c r="B79" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E79" s="0" t="n">
+      <c r="D79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="1" t="n">
         <v>9.4</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F79" s="1" t="n">
         <v>25.9</v>
       </c>
     </row>
@@ -1765,16 +1766,16 @@
       <c r="B80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" s="0" t="n">
+      <c r="D80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="1" t="n">
         <v>10.4</v>
       </c>
-      <c r="F80" s="0" t="n">
+      <c r="F80" s="1" t="n">
         <v>29.5</v>
       </c>
     </row>
@@ -1785,16 +1786,16 @@
       <c r="B81" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D81" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E81" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F81" s="0" t="n">
+      <c r="D81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="F81" s="1" t="n">
         <v>30.3</v>
       </c>
     </row>
@@ -1802,419 +1803,419 @@
       <c r="A82" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="0" t="n">
+      <c r="B82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D82" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E82" s="0" t="n">
+      <c r="D82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F82" s="1" t="n">
         <v>24</v>
-      </c>
-      <c r="F82" s="0" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B83" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" s="0" t="n">
+      <c r="B83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="F83" s="1" t="n">
         <v>21</v>
-      </c>
-      <c r="F83" s="0" t="n">
-        <v>4.9</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="0" t="n">
+      <c r="B84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E84" s="0" t="n">
+      <c r="E84" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F84" s="1" t="n">
         <v>19</v>
-      </c>
-      <c r="F84" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="0" t="n">
+      <c r="B85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F85" s="1" t="n">
         <v>21</v>
-      </c>
-      <c r="F85" s="0" t="n">
-        <v>4.2</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="0" t="n">
+      <c r="B86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E86" s="0" t="n">
+      <c r="E86" s="1" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="F86" s="1" t="n">
         <v>21</v>
-      </c>
-      <c r="F86" s="0" t="n">
-        <v>3.8</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="0" t="n">
+      <c r="B87" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E87" s="0" t="n">
+      <c r="E87" s="1" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="F87" s="1" t="n">
         <v>19.4</v>
-      </c>
-      <c r="F87" s="0" t="n">
-        <v>4.4</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="0" t="n">
+      <c r="B88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E88" s="0" t="n">
+      <c r="E88" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="F88" s="1" t="n">
         <v>24.6</v>
-      </c>
-      <c r="F88" s="0" t="n">
-        <v>4.9</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C89" s="0" t="n">
+      <c r="B89" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="1" t="n">
         <v>8</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F89" s="1" t="n">
         <v>23</v>
-      </c>
-      <c r="F89" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B90" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="0" t="n">
+      <c r="B90" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="1" t="n">
         <v>9</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E90" s="0" t="n">
+      <c r="E90" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F90" s="1" t="n">
         <v>22.9</v>
-      </c>
-      <c r="F90" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B91" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C91" s="0" t="n">
+      <c r="B91" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E91" s="0" t="n">
+      <c r="E91" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F91" s="1" t="n">
         <v>21</v>
-      </c>
-      <c r="F91" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" s="0" t="n">
+      <c r="B92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="1" t="n">
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E92" s="0" t="n">
+      <c r="E92" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="F92" s="1" t="n">
         <v>24.1</v>
-      </c>
-      <c r="F92" s="0" t="n">
-        <v>4.9</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B93" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C93" s="0" t="n">
+      <c r="B93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="1" t="n">
         <v>11</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E93" s="0" t="n">
+      <c r="E93" s="1" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="F93" s="1" t="n">
         <v>10.16</v>
-      </c>
-      <c r="F93" s="0" t="n">
-        <v>3.9</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B94" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" s="0" t="n">
+      <c r="B94" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="1" t="n">
         <v>12</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="0" t="n">
+      <c r="E94" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="F94" s="1" t="n">
         <v>20.3</v>
-      </c>
-      <c r="F94" s="0" t="n">
-        <v>4.9</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C95" s="0" t="n">
+      <c r="B95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="1" t="n">
         <v>13</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E95" s="0" t="n">
+      <c r="E95" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="F95" s="1" t="n">
         <v>22</v>
-      </c>
-      <c r="F95" s="0" t="n">
-        <v>5.6</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B96" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="0" t="n">
+      <c r="B96" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" s="1" t="n">
         <v>14</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E96" s="0" t="n">
+      <c r="E96" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F96" s="1" t="n">
         <v>4.6</v>
-      </c>
-      <c r="F96" s="0" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C97" s="0" t="n">
+      <c r="B97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="1" t="n">
         <v>15</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E97" s="0" t="n">
+      <c r="E97" s="1" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="F97" s="1" t="n">
         <v>18.3</v>
-      </c>
-      <c r="F97" s="0" t="n">
-        <v>4.6</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B98" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C98" s="0" t="n">
+      <c r="B98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="1" t="n">
         <v>16</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E98" s="0" t="n">
+      <c r="E98" s="1" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F98" s="1" t="n">
         <v>20.2</v>
-      </c>
-      <c r="F98" s="0" t="n">
-        <v>3.7</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="0" t="n">
+      <c r="B99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E99" s="0" t="n">
+      <c r="E99" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F99" s="1" t="n">
         <v>7.8</v>
-      </c>
-      <c r="F99" s="0" t="n">
-        <v>4.2</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B100" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C100" s="0" t="n">
+      <c r="B100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="1" t="n">
         <v>19</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E100" s="0" t="n">
+      <c r="E100" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F100" s="1" t="n">
         <v>21.5</v>
-      </c>
-      <c r="F100" s="0" t="n">
-        <v>4.2</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B101" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" s="0" t="n">
+      <c r="B101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="1" t="n">
         <v>20</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E101" s="0" t="n">
+      <c r="E101" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F101" s="1" t="n">
         <v>20.5</v>
-      </c>
-      <c r="F101" s="0" t="n">
-        <v>4.8</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C102" s="0" t="n">
+      <c r="B102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D102" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E102" s="0" t="n">
+      <c r="D102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E102" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="F102" s="0" t="n">
+      <c r="F102" s="1" t="n">
         <v>24</v>
       </c>
     </row>
@@ -2225,16 +2226,16 @@
       <c r="B103" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C103" s="0" t="n">
+      <c r="C103" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D103" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E103" s="0" t="n">
+      <c r="D103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F103" s="0" t="n">
+      <c r="F103" s="1" t="n">
         <v>10.7</v>
       </c>
     </row>
@@ -2245,16 +2246,16 @@
       <c r="B104" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C104" s="0" t="n">
+      <c r="C104" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D104" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E104" s="0" t="n">
+      <c r="D104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F104" s="0" t="n">
+      <c r="F104" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2265,16 +2266,16 @@
       <c r="B105" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="0" t="n">
+      <c r="C105" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D105" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E105" s="0" t="n">
+      <c r="D105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F105" s="0" t="n">
+      <c r="F105" s="1" t="n">
         <v>22.4</v>
       </c>
     </row>
@@ -2285,16 +2286,16 @@
       <c r="B106" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C106" s="0" t="n">
+      <c r="C106" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D106" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E106" s="0" t="n">
+      <c r="D106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="F106" s="0" t="n">
+      <c r="F106" s="1" t="n">
         <v>10.6</v>
       </c>
     </row>
@@ -2305,16 +2306,16 @@
       <c r="B107" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C107" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D107" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E107" s="0" t="n">
+      <c r="C107" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107" s="1" t="n">
         <v>4.4</v>
       </c>
-      <c r="F107" s="0" t="n">
+      <c r="F107" s="1" t="n">
         <v>22.1</v>
       </c>
     </row>
@@ -2325,16 +2326,16 @@
       <c r="B108" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C108" s="0" t="n">
+      <c r="C108" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D108" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E108" s="0" t="n">
+      <c r="D108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E108" s="1" t="n">
         <v>3.7</v>
       </c>
-      <c r="F108" s="0" t="n">
+      <c r="F108" s="1" t="n">
         <v>20.5</v>
       </c>
     </row>
@@ -2345,16 +2346,16 @@
       <c r="B109" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C109" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D109" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E109" s="0" t="n">
+      <c r="C109" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E109" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="F109" s="0" t="n">
+      <c r="F109" s="1" t="n">
         <v>10.18</v>
       </c>
     </row>
@@ -2365,16 +2366,16 @@
       <c r="B110" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C110" s="0" t="n">
+      <c r="C110" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D110" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E110" s="0" t="n">
+      <c r="D110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" s="1" t="n">
         <v>4.3</v>
       </c>
-      <c r="F110" s="0" t="n">
+      <c r="F110" s="1" t="n">
         <v>20.01</v>
       </c>
     </row>
@@ -2385,16 +2386,16 @@
       <c r="B111" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C111" s="0" t="n">
+      <c r="C111" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D111" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E111" s="0" t="n">
+      <c r="D111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E111" s="1" t="n">
         <v>5.2</v>
       </c>
-      <c r="F111" s="0" t="n">
+      <c r="F111" s="1" t="n">
         <v>20.3</v>
       </c>
     </row>
@@ -2405,16 +2406,16 @@
       <c r="B112" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C112" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E112" s="0" t="n">
+      <c r="C112" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F112" s="0" t="n">
+      <c r="F112" s="1" t="n">
         <v>20.4</v>
       </c>
     </row>
@@ -2425,16 +2426,16 @@
       <c r="B113" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" s="0" t="n">
+      <c r="C113" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F113" s="0" t="n">
+      <c r="F113" s="1" t="n">
         <v>20.1</v>
       </c>
     </row>
@@ -2445,16 +2446,16 @@
       <c r="B114" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C114" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E114" s="0" t="n">
+      <c r="C114" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F114" s="0" t="n">
+      <c r="F114" s="1" t="n">
         <v>17</v>
       </c>
     </row>
@@ -2465,16 +2466,16 @@
       <c r="B115" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C115" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D115" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115" s="0" t="n">
+      <c r="C115" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F115" s="0" t="n">
+      <c r="F115" s="1" t="n">
         <v>21</v>
       </c>
     </row>
@@ -2485,16 +2486,16 @@
       <c r="B116" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C116" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E116" s="0" t="n">
+      <c r="C116" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="F116" s="0" t="n">
+      <c r="F116" s="1" t="n">
         <v>22</v>
       </c>
     </row>
@@ -2505,16 +2506,16 @@
       <c r="B117" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C117" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E117" s="0" t="n">
+      <c r="C117" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" s="1" t="n">
         <v>4.4</v>
       </c>
-      <c r="F117" s="0" t="n">
+      <c r="F117" s="1" t="n">
         <v>10.19</v>
       </c>
     </row>
@@ -2525,16 +2526,16 @@
       <c r="B118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C118" s="0" t="n">
+      <c r="C118" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="D118" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E118" s="0" t="n">
+      <c r="D118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F118" s="0" t="n">
+      <c r="F118" s="1" t="n">
         <v>24</v>
       </c>
     </row>
@@ -2545,16 +2546,16 @@
       <c r="B119" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C119" s="0" t="n">
+      <c r="C119" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D119" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E119" s="0" t="n">
+      <c r="D119" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" s="1" t="n">
         <v>5.6</v>
       </c>
-      <c r="F119" s="0" t="n">
+      <c r="F119" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2565,16 +2566,16 @@
       <c r="B120" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C120" s="0" t="n">
+      <c r="C120" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D120" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E120" s="0" t="n">
+      <c r="D120" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" s="1" t="n">
         <v>3.7</v>
       </c>
-      <c r="F120" s="0" t="n">
+      <c r="F120" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2585,16 +2586,16 @@
       <c r="B121" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C121" s="0" t="n">
+      <c r="C121" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D121" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E121" s="0" t="n">
+      <c r="D121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" s="1" t="n">
         <v>4.4</v>
       </c>
-      <c r="F121" s="0" t="n">
+      <c r="F121" s="1" t="n">
         <v>20.05</v>
       </c>
     </row>

</xml_diff>